<commit_message>
Updated figure and removed todo's section 2
</commit_message>
<xml_diff>
--- a/Paper/ECAI/figures/Demo.xlsx
+++ b/Paper/ECAI/figures/Demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -179,31 +179,34 @@
     <t>B6 = T2[1:4,:]</t>
   </si>
   <si>
-    <t>B7 = T3[:,1]</t>
-  </si>
-  <si>
-    <t>B8 = T3[:,2]</t>
-  </si>
-  <si>
-    <t>B9 = T4[:,1]</t>
-  </si>
-  <si>
-    <t>B15 = T6[:,2:4]</t>
-  </si>
-  <si>
-    <t>B14 = T5[:,1]</t>
-  </si>
-  <si>
-    <t>B13 = T5[:,2]</t>
-  </si>
-  <si>
-    <t>B12 = T5[:,1]</t>
-  </si>
-  <si>
-    <t>B11 = T4[:,3]</t>
-  </si>
-  <si>
-    <t>B10 = T4[:,2]</t>
+    <t>B7 = T2[1:4,:]</t>
+  </si>
+  <si>
+    <t>B8 = T3[:,1]</t>
+  </si>
+  <si>
+    <t>B9 = T3[:,2]</t>
+  </si>
+  <si>
+    <t>B10 = T4[:,1]</t>
+  </si>
+  <si>
+    <t>B11 = T4[:,2]</t>
+  </si>
+  <si>
+    <t>B12 = T4[:,3]</t>
+  </si>
+  <si>
+    <t>B13 = T5[:,1]</t>
+  </si>
+  <si>
+    <t>B14 = T5[:,2]</t>
+  </si>
+  <si>
+    <t>B15 = T5[:,1]</t>
+  </si>
+  <si>
+    <t>B16 = T6[:,2:4]</t>
   </si>
 </sst>
 </file>
@@ -262,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -311,9 +314,7 @@
       <left style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
+      <right/>
       <top style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </top>
@@ -321,12 +322,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
+      <left/>
+      <right/>
       <top style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </top>
@@ -334,9 +331,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
+      <left/>
       <right style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </right>
@@ -350,28 +345,13 @@
       <left style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
+      <left/>
       <right style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </right>
@@ -383,50 +363,9 @@
       <left style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
         <color theme="9" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
@@ -434,10 +373,8 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
@@ -447,83 +384,7 @@
       <right style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </right>
-      <top style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color theme="9" tint="-0.24994659260841701"/>
       </bottom>
@@ -533,9 +394,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -575,16 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,10 +748,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -919,120 +774,120 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="18">
         <v>353</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="19">
         <v>378</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="19">
         <v>396</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="19">
         <v>387</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="19">
         <v>1514</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="20">
         <v>2</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="18">
         <v>34</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="20">
         <v>20</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="21">
         <v>370</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="2">
         <v>408</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="2">
         <v>387</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="2">
         <v>386</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="2">
         <v>1551</v>
       </c>
       <c r="H3" s="22">
         <v>1</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="21">
         <v>29</v>
       </c>
       <c r="K3" s="22">
         <v>10</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="21">
         <v>175</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="2">
         <v>146</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="2">
         <v>167</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="2">
         <v>203</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="2">
         <v>691</v>
       </c>
       <c r="H4" s="22">
         <v>3</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="21">
         <v>19</v>
       </c>
       <c r="K4" s="22">
         <v>19</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="23">
@@ -1053,7 +908,7 @@
       <c r="H5" s="25">
         <v>4</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="23">
@@ -1062,436 +917,458 @@
       <c r="K5" s="25">
         <v>15</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="5" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" spans="1:12" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C9" s="18">
         <v>991</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D9" s="19">
         <v>1030</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E9" s="19">
         <v>1046</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F9" s="19">
         <v>1081</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G9" s="20">
         <v>4148</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="29">
-        <v>247.75</v>
-      </c>
-      <c r="D9" s="30">
-        <v>257.5</v>
-      </c>
-      <c r="E9" s="30">
-        <v>261.5</v>
-      </c>
-      <c r="F9" s="30">
-        <v>270.25</v>
-      </c>
-      <c r="G9" s="31">
-        <v>1037</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="J9" s="14">
-        <v>0</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="21">
+        <v>247.75</v>
+      </c>
+      <c r="D10" s="2">
+        <v>257.5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>261.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>270.25</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1037</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="J10" s="15">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C11" s="21">
         <v>370</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D11" s="2">
         <v>408</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E11" s="2">
         <v>396</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F11" s="2">
         <v>387</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G11" s="22">
         <v>1551</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="J10" s="15">
+      <c r="H11" s="10"/>
+      <c r="J11" s="16">
         <v>0.8</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C12" s="23">
         <v>93</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D12" s="24">
         <v>98</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E12" s="24">
         <v>96</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F12" s="24">
         <v>105</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G12" s="25">
         <v>392</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="J11" s="16">
+      <c r="H12" s="10"/>
+      <c r="J12" s="17">
         <v>1.2</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="J12" s="7" t="s">
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="J13" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="K13" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="11">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="11">
-        <v>5</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="12">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C17" s="13">
         <v>3</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="H16" s="12" t="s">
+      <c r="E17" s="4"/>
+      <c r="H17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I17" s="13">
         <v>10</v>
       </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C18" s="13">
         <v>3</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="H17" s="12" t="s">
+      <c r="E18" s="4"/>
+      <c r="H18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I18" s="13">
         <v>8</v>
       </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C19" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="H18" s="12" t="s">
+      <c r="E19" s="4"/>
+      <c r="H19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I19" s="13">
         <v>9</v>
       </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C20" s="14">
         <v>4</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="H19" s="12" t="s">
+      <c r="E20" s="4"/>
+      <c r="H20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I20" s="13">
         <v>15</v>
       </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="13">
+        <v>8</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="13">
+        <v>2</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="13">
+        <v>20</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="18">
+        <v>991</v>
+      </c>
+      <c r="D24" s="19">
+        <v>212</v>
+      </c>
+      <c r="E24" s="20">
+        <v>779</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="13">
+        <v>3</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="21">
+        <v>1030</v>
+      </c>
+      <c r="D25" s="2">
+        <v>710</v>
+      </c>
+      <c r="E25" s="22">
+        <v>1099</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="H25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="14">
+        <v>19</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1046</v>
+      </c>
+      <c r="D26" s="2">
+        <v>137</v>
+      </c>
+      <c r="E26" s="22">
+        <v>2008</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="H26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="23">
+        <v>1081</v>
+      </c>
+      <c r="D27" s="24">
+        <v>240</v>
+      </c>
+      <c r="E27" s="25">
+        <v>2849</v>
+      </c>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="12">
-        <v>8</v>
-      </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H21" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="12">
-        <v>2</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="12">
-        <v>20</v>
-      </c>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="17">
-        <v>991</v>
-      </c>
-      <c r="D23" s="18">
-        <v>212</v>
-      </c>
-      <c r="E23" s="19">
-        <v>779</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="12">
-        <v>3</v>
-      </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="20">
-        <v>1030</v>
-      </c>
-      <c r="D24" s="21">
-        <v>710</v>
-      </c>
-      <c r="E24" s="22">
-        <v>1099</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="H24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="13">
-        <v>19</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="20">
-        <v>1046</v>
-      </c>
-      <c r="D25" s="21">
-        <v>137</v>
-      </c>
-      <c r="E25" s="22">
-        <v>2008</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="H25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="23">
-        <v>1081</v>
-      </c>
-      <c r="D26" s="24">
-        <v>240</v>
-      </c>
-      <c r="E26" s="25">
-        <v>2849</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="C28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E15:E19"/>
+  <mergeCells count="11">
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="C8:G8"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="C28:E28"/>
     <mergeCell ref="L2:L5"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="J15:J24"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="J16:J25"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="F24:F27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="27" max="16383" man="1"/>
+    <brk id="28" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="12" max="1048575" man="1"/>

</xml_diff>

<commit_message>
Updated paper and figures
</commit_message>
<xml_diff>
--- a/Paper/ECAI/figures/Demo.xlsx
+++ b/Paper/ECAI/figures/Demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -152,46 +152,43 @@
     <t>T4</t>
   </si>
   <si>
-    <t>B1 = T1[:,1]</t>
-  </si>
-  <si>
-    <t>B2 = T1[:,2]</t>
-  </si>
-  <si>
-    <t>B3 = T1[:,3:8]</t>
-  </si>
-  <si>
-    <t>B4 = T1[:,9]</t>
-  </si>
-  <si>
-    <t>B5 = T1[:,10:11]</t>
-  </si>
-  <si>
-    <t>B6 = T2[1:4,:]</t>
-  </si>
-  <si>
-    <t>B7 = T2[1:4,:]</t>
-  </si>
-  <si>
-    <t>B8 = T3[:,1]</t>
-  </si>
-  <si>
-    <t>B9 = T3[:,2]</t>
-  </si>
-  <si>
-    <t>B10 = T4[:,1]</t>
-  </si>
-  <si>
-    <t>B14 = T5[:,3]</t>
-  </si>
-  <si>
-    <t>B13 = T5[:,2]</t>
-  </si>
-  <si>
-    <t>B12 = T5[:,1]</t>
-  </si>
-  <si>
-    <t>B11 = T4[:,2:4]</t>
+    <t>B1 = T1[:, 1]</t>
+  </si>
+  <si>
+    <t>B2 = T1[:, 2]</t>
+  </si>
+  <si>
+    <t>B3 = T1[:, 3:8]</t>
+  </si>
+  <si>
+    <t>B4 = T1[:, 9]</t>
+  </si>
+  <si>
+    <t>B5 = T1[:, 10:11]</t>
+  </si>
+  <si>
+    <t>B6 = T2[1:4, :]</t>
+  </si>
+  <si>
+    <t>B8 = T3[:, 1]</t>
+  </si>
+  <si>
+    <t>B9 = T3[:, 2]</t>
+  </si>
+  <si>
+    <t>B14 = T5[:, 3]</t>
+  </si>
+  <si>
+    <t>B13 = T5[:, 2]</t>
+  </si>
+  <si>
+    <t>B12 = T5[:, 1]</t>
+  </si>
+  <si>
+    <t>B11 = T4[:, 2:4]</t>
+  </si>
+  <si>
+    <t>B10 = T4[:, 1]</t>
   </si>
 </sst>
 </file>
@@ -379,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -404,8 +401,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,12 +415,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,12 +704,12 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -787,7 +791,7 @@
       <c r="K2" s="11">
         <v>20</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -825,7 +829,7 @@
       <c r="K3" s="13">
         <v>10</v>
       </c>
-      <c r="L3" s="18"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
@@ -861,7 +865,7 @@
       <c r="K4" s="13">
         <v>19</v>
       </c>
-      <c r="L4" s="18"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -897,7 +901,7 @@
       <c r="K5" s="16">
         <v>15</v>
       </c>
-      <c r="L5" s="18"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -906,21 +910,21 @@
       <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -969,7 +973,7 @@
       <c r="G9" s="11">
         <v>4148</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="23" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="6" t="s">
@@ -978,7 +982,7 @@
       <c r="K9" s="6">
         <v>5</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="20" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1001,14 +1005,14 @@
       <c r="G10" s="13">
         <v>1037</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="23"/>
       <c r="J10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="7">
         <v>10</v>
       </c>
-      <c r="L10" s="18"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -1029,14 +1033,14 @@
       <c r="G11" s="13">
         <v>1551</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="23"/>
       <c r="J11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K11" s="7">
         <v>8</v>
       </c>
-      <c r="L11" s="18"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1057,62 +1061,87 @@
       <c r="G12" s="16">
         <v>392</v>
       </c>
-      <c r="H12" s="20"/>
+      <c r="H12" s="23"/>
       <c r="J12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="7">
         <v>9</v>
       </c>
-      <c r="L12" s="18"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="18"/>
       <c r="J13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K13" s="7">
         <v>15</v>
       </c>
-      <c r="L13" s="18"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="7">
         <v>8</v>
       </c>
-      <c r="L14" s="18"/>
-    </row>
-    <row r="15" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
+      <c r="L14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="9">
+        <v>991</v>
+      </c>
+      <c r="C15" s="10">
+        <v>212</v>
+      </c>
+      <c r="D15" s="11">
+        <v>779</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>16</v>
@@ -1120,60 +1149,56 @@
       <c r="K15" s="7">
         <v>2</v>
       </c>
-      <c r="L15" s="18"/>
+      <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="9">
-        <v>991</v>
-      </c>
-      <c r="C16" s="10">
-        <v>212</v>
-      </c>
-      <c r="D16" s="11">
-        <v>779</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>38</v>
-      </c>
+      <c r="A16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1030</v>
+      </c>
+      <c r="C16" s="2">
+        <v>710</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1099</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="26"/>
       <c r="J16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="7">
         <v>20</v>
       </c>
-      <c r="L16" s="18"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="12">
-        <v>1030</v>
+        <v>1046</v>
       </c>
       <c r="C17" s="2">
-        <v>710</v>
+        <v>137</v>
       </c>
       <c r="D17" s="13">
-        <v>1099</v>
-      </c>
-      <c r="E17" s="18"/>
+        <v>2008</v>
+      </c>
+      <c r="E17" s="25"/>
       <c r="F17" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="7">
         <v>3</v>
@@ -1181,121 +1206,96 @@
       <c r="H17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="18"/>
+      <c r="I17" s="26"/>
       <c r="J17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K17" s="7">
         <v>3</v>
       </c>
-      <c r="L17" s="18"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="12">
-        <v>1046</v>
-      </c>
-      <c r="C18" s="2">
-        <v>137</v>
-      </c>
-      <c r="D18" s="13">
-        <v>2008</v>
-      </c>
-      <c r="E18" s="18"/>
+      <c r="A18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="14">
+        <v>1081</v>
+      </c>
+      <c r="C18" s="15">
+        <v>240</v>
+      </c>
+      <c r="D18" s="16">
+        <v>2849</v>
+      </c>
+      <c r="E18" s="25"/>
       <c r="F18" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="I18" s="26"/>
       <c r="J18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K18" s="8">
         <v>19</v>
       </c>
-      <c r="L18" s="18"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="14">
-        <v>1081</v>
-      </c>
-      <c r="C19" s="15">
-        <v>240</v>
-      </c>
-      <c r="D19" s="16">
-        <v>2849</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="7">
-        <v>2</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="18"/>
+      <c r="A19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="F19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="8">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="26"/>
       <c r="J19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="5" t="s">
+    </row>
+    <row r="20" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="F20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="8">
-        <v>4</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
+    <row r="21" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B20:D20"/>
+  <mergeCells count="9">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="I15:I19"/>
     <mergeCell ref="L2:L5"/>
     <mergeCell ref="L9:L18"/>
-    <mergeCell ref="E16:E19"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="I16:I20"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="H9:H12"/>
@@ -1304,7 +1304,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="21" max="16383" man="1"/>
+    <brk id="20" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="12" max="1048575" man="1"/>

</xml_diff>